<commit_message>
First version of SOA as qmd
</commit_message>
<xml_diff>
--- a/data/uac_glossary.xlsx
+++ b/data/uac_glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA84DA3-B2E0-8F4A-9455-9AA285B2B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EEC763-291B-F945-939E-81EF714ACF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60980" yWindow="-30220" windowWidth="57600" windowHeight="30600" xr2:uid="{FD61D8A1-D7A7-6B4D-AB92-59721C5EF8F9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FD61D8A1-D7A7-6B4D-AB92-59721C5EF8F9}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <t>Topic</t>
   </si>
@@ -288,6 +288,39 @@
   </si>
   <si>
     <t>Depth of field in photography refers to the range of distances in an image where objects appear acceptably sharp and in focus, controlled by factors such as aperture size and focal length.</t>
+  </si>
+  <si>
+    <t>Amplifier</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Channel aka Strip</t>
+  </si>
+  <si>
+    <t>Direct Box</t>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An audio component that take low-level inputs, from a console, and amplifies them to the power level required to drive a speaker. </t>
+  </si>
+  <si>
+    <t>Refers to a logical structure within the console where multiple channels (sources) can contribute an audio signal.</t>
+  </si>
+  <si>
+    <t>Refers to an input in the console. Typically this is a microphone input or an instrument.</t>
+  </si>
+  <si>
+    <t>A device, usually a box, which can interface an instrument, like a electronic keyboard, to an audio console.</t>
+  </si>
+  <si>
+    <t>A collection of setting which can be saved and recalled as a group.</t>
   </si>
 </sst>
 </file>
@@ -350,8 +383,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}" name="Table1" displayName="Table1" ref="A1:D39" totalsRowShown="0">
-  <autoFilter ref="A1:D39" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}" name="Table1" displayName="Table1" ref="A1:D53" totalsRowShown="0">
+  <autoFilter ref="A1:D53" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
     <sortCondition ref="A2:A35"/>
     <sortCondition ref="B2:B35"/>
@@ -663,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B4C12-DB51-F04E-97D5-67343BD74C6D}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="282" zoomScaleNormal="282" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="282" zoomScaleNormal="282" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,6 +1152,88 @@
         <v>83</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Major revisions to SDL
</commit_message>
<xml_diff>
--- a/data/uac_glossary.xlsx
+++ b/data/uac_glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F47957-A73E-3644-B05B-2850429E3BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94503DD1-DB6A-2441-8F9E-995D154C44EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-65360" yWindow="-29000" windowWidth="63400" windowHeight="32220" xr2:uid="{FD61D8A1-D7A7-6B4D-AB92-59721C5EF8F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="111">
   <si>
     <t>Topic</t>
   </si>
@@ -339,6 +339,36 @@
   </si>
   <si>
     <t>A general classification of cabling that is often used for networks, but can also be used for video (see *HDBaseT*),* DMX*, or audio. There are several 'categories' in common use, eg cat5e, and cat6.</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Nema L2-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power </t>
+  </si>
+  <si>
+    <t>This is a heavy duty 20 Amp  connector with circular locking contacts  (hence the **L** in the name). There is an *R* and a *P* suffix for the *recepacle* and *plug*.</t>
+  </si>
+  <si>
+    <t>This is a regular three-prong   connector  good for 15 Amps . There is an *R* and a *P* suffix for the *recepacle* and *plug*.</t>
+  </si>
+  <si>
+    <t>Nema 5-15</t>
+  </si>
+  <si>
+    <t>Nema 6-20</t>
+  </si>
+  <si>
+    <t>This looks like a regular three-prong plug but one of the blades is turned 90 degrees. This connector is good for 20 Amp.  There is an *R* and a *P* suffix for the *recepacle* and *plug*.</t>
+  </si>
+  <si>
+    <t>Cam-Lock</t>
+  </si>
+  <si>
+    <t>A power connector type used for large current power distribution (&gt; 100 Amp). See https://en.wikipedia.org/wiki/Camlock_(electrical)</t>
   </si>
 </sst>
 </file>
@@ -416,8 +446,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}" name="Table1" displayName="Table1" ref="A1:D46" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D46" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}" name="Table1" displayName="Table1" ref="A1:D50" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D50" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
     <sortCondition ref="A2:A26"/>
     <sortCondition ref="B2:B26"/>
@@ -729,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B4C12-DB51-F04E-97D5-67343BD74C6D}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,6 +1337,54 @@
         <v>99</v>
       </c>
     </row>
+    <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
revisions to sda for new audio sys
</commit_message>
<xml_diff>
--- a/data/uac_glossary.xlsx
+++ b/data/uac_glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94503DD1-DB6A-2441-8F9E-995D154C44EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF7B3CC-FBFC-4F40-BA4D-80964C87E012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-65360" yWindow="-29000" windowWidth="63400" windowHeight="32220" xr2:uid="{FD61D8A1-D7A7-6B4D-AB92-59721C5EF8F9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FD61D8A1-D7A7-6B4D-AB92-59721C5EF8F9}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="115">
   <si>
     <t>Topic</t>
   </si>
@@ -369,6 +369,18 @@
   </si>
   <si>
     <t>A power connector type used for large current power distribution (&gt; 100 Amp). See https://en.wikipedia.org/wiki/Camlock_(electrical)</t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>A video (and audio) transport protocol which operates over COAX cable.</t>
+  </si>
+  <si>
+    <t>STP</t>
+  </si>
+  <si>
+    <t>Sheilded Twisted Pair - a type of cable that has shield which encases the twisted pairs.</t>
   </si>
 </sst>
 </file>
@@ -446,11 +458,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}" name="Table1" displayName="Table1" ref="A1:D50" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D50" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
-    <sortCondition ref="A2:A26"/>
-    <sortCondition ref="B2:B26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}" name="Table1" displayName="Table1" ref="A1:D52" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D52" xr:uid="{314A4941-A8BA-2346-8EA0-5892B4F1C3B7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D52">
+    <sortCondition ref="A2:A52"/>
+    <sortCondition ref="B2:B52"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A991846A-4384-6048-992B-FAECE1424BD1}" name="Topic" dataDxfId="3"/>
@@ -463,9 +475,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -503,7 +515,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -609,7 +621,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -751,7 +763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B4C12-DB51-F04E-97D5-67343BD74C6D}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,604 +797,628 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="2" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="D35" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C40" s="1"/>
       <c r="D40" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D41" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="2" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="2" t="s">
-        <v>110</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>